<commit_message>
Added in the user model and some database middleware.
</commit_message>
<xml_diff>
--- a/SoloProjectUserStories.xlsx
+++ b/SoloProjectUserStories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PalmTreeRecipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stink\Documents\PalmTreeRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{476821BC-B1E4-4A17-8124-440BE0055CB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55185D1E-4A94-4179-9762-212BF7CB2E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{3A16AFFF-6FA6-4208-BECC-4321666F3CEE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A16AFFF-6FA6-4208-BECC-4321666F3CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,179 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+  <si>
+    <t>I want to…</t>
+  </si>
+  <si>
+    <t>Because…</t>
+  </si>
+  <si>
+    <t>As A…</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>User/ Administrator</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>I want to access my account</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>I want to create an account</t>
+  </si>
+  <si>
+    <t>View my profile</t>
+  </si>
+  <si>
+    <t>I want to see my information</t>
+  </si>
+  <si>
+    <t>Update my profile</t>
+  </si>
+  <si>
+    <t>I want to update my information</t>
+  </si>
+  <si>
+    <t>Delete my profile</t>
+  </si>
+  <si>
+    <t>I don't want to be a part of the site</t>
+  </si>
+  <si>
+    <t>Search recipes</t>
+  </si>
+  <si>
+    <t>I can find the recipe I’m looking for</t>
+  </si>
+  <si>
+    <t>User/. Guest</t>
+  </si>
+  <si>
+    <t>View recipes</t>
+  </si>
+  <si>
+    <t>I can cook the recipe</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>View all profiles</t>
+  </si>
+  <si>
+    <t>I can see all the users</t>
+  </si>
+  <si>
+    <t>Update a profile</t>
+  </si>
+  <si>
+    <t>I may need to change the content of the profile</t>
+  </si>
+  <si>
+    <t>Delete a profile</t>
+  </si>
+  <si>
+    <t>I don't want the user on my site</t>
+  </si>
+  <si>
+    <t>Update a recipe</t>
+  </si>
+  <si>
+    <t>I may need to change the content of the recipe</t>
+  </si>
+  <si>
+    <t>Gues</t>
+  </si>
+  <si>
+    <t>Lock out profiles</t>
+  </si>
+  <si>
+    <t>I don't want a guest to be able to view profiles</t>
+  </si>
+  <si>
+    <t>Create a recipe</t>
+  </si>
+  <si>
+    <t>I want to add my recipe to the site</t>
+  </si>
+  <si>
+    <t>Update my recipes</t>
+  </si>
+  <si>
+    <t>I want to change the content of my recipes</t>
+  </si>
+  <si>
+    <t>Delete my recipes</t>
+  </si>
+  <si>
+    <t>I want to remove my recipe from the site</t>
+  </si>
+  <si>
+    <t>Print recipes out</t>
+  </si>
+  <si>
+    <t>I want to be able to get a physical copy of a recipe</t>
+  </si>
+  <si>
+    <t>Review Recipes</t>
+  </si>
+  <si>
+    <t>I want to leave feedback on a recipe</t>
+  </si>
+  <si>
+    <t>Comment on a recipe</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +220,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +537,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7E1819-79BD-406B-9ADA-26563B8AADCD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:E20">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>